<commit_message>
Umbau auf normale SQL Conn
</commit_message>
<xml_diff>
--- a/bosnjak_protokoll.xlsx
+++ b/bosnjak_protokoll.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Datum</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>Creates, Inserts, View</t>
+  </si>
+  <si>
+    <t>ListView, Database Connection</t>
+  </si>
+  <si>
+    <t>Database Connection</t>
   </si>
 </sst>
 </file>
@@ -89,11 +95,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -371,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,6 +464,42 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>42395</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.73055555555555562</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.75694444444444453</v>
+      </c>
+      <c r="D5" s="3">
+        <f>C5-B5</f>
+        <v>2.6388888888888906E-2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>42395</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.77430555555555547</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.80347222222222225</v>
+      </c>
+      <c r="D6" s="3">
+        <f>C6-B6</f>
+        <v>2.9166666666666785E-2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Aenderung des SQL Accountes
</commit_message>
<xml_diff>
--- a/bosnjak_protokoll.xlsx
+++ b/bosnjak_protokoll.xlsx
@@ -62,7 +62,7 @@
     <t>Databinding</t>
   </si>
   <si>
-    <t>neu erstellen</t>
+    <t>neu erstellen, grid funktioniert, Button erstellt</t>
   </si>
 </sst>
 </file>
@@ -387,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -430,7 +430,7 @@
         <v>0.77013888888888893</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D8" si="0">C2-B2</f>
+        <f t="shared" ref="D2:D9" si="0">C2-B2</f>
         <v>2.2916666666666696E-2</v>
       </c>
       <c r="E2" t="s">
@@ -552,9 +552,19 @@
       <c r="B9" s="3">
         <v>0.66736111111111107</v>
       </c>
+      <c r="C9" s="3">
+        <v>0.7631944444444444</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>9.5833333333333326E-2</v>
+      </c>
       <c r="E9" t="s">
         <v>12</v>
       </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>